<commit_message>
Update V-King CoreXY V2 - Part Order List.xlsx
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/V-King CoreXY V2 - Part Order List.xlsx
+++ b/Document Library/Bill Of Materials/V-King CoreXY V2 - Part Order List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-King CoreXY/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="632" documentId="6_{B6BB48D1-6332-477D-B7B9-3E9DE76C918E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{839B0EB5-D140-49FE-A8FE-0D49C5DA7EC7}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="6_{B6BB48D1-6332-477D-B7B9-3E9DE76C918E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C4C6CD43-ABC7-4FBE-A4E1-048DF3FED81E}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,15 +883,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -925,6 +916,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1763,44 +1763,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3"/>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1906,33 +1906,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="69"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="27">
-      <c r="A2" s="64"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="73" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="68"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="74"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="75"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="46" t="s">
@@ -1943,11 +1943,11 @@
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
-      <c r="E4" s="59">
+      <c r="E4" s="56">
         <v>345</v>
       </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -1968,10 +1968,10 @@
       <c r="E5" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2546,7 +2546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407AFBB0-CFB7-4080-B7E4-F71BBADF622E}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -3082,6 +3084,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>